<commit_message>
snowflake test cases updated
</commit_message>
<xml_diff>
--- a/test/testcases/testcase23_parquet_snowflake_mismatch.xlsx
+++ b/test/testcases/testcase23_parquet_snowflake_mismatch.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_Automated_Testing_Framework\test\testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE34E0C-316C-40D5-A8CB-3FF91FF700DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C361F73-F5BD-42EA-8675-C496F035A0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>sourcequerymode</t>
   </si>
@@ -144,12 +144,6 @@
     <t>table</t>
   </si>
   <si>
-    <t>patients_db</t>
-  </si>
-  <si>
-    <t>patients</t>
-  </si>
-  <si>
     <t>BIRTHDATE,DEATHDATE</t>
   </si>
   <si>
@@ -178,6 +172,9 @@
   </si>
   <si>
     <t>RawS3Parquet</t>
+  </si>
+  <si>
+    <t>SAMPLE_SRC_PATIENTS</t>
   </si>
 </sst>
 </file>
@@ -557,7 +554,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +602,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -613,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -621,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -629,7 +626,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -637,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -663,7 +660,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -706,7 +703,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -721,16 +718,14 @@
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -755,7 +750,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>